<commit_message>
Fri Oct 27 06:19:42 PM CST 2023
</commit_message>
<xml_diff>
--- a/lixiao/performance_2023_10/assess_绩效+软性考核表.xlsx
+++ b/lixiao/performance_2023_10/assess_绩效+软性考核表.xlsx
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
   <si>
     <t>绩效考核汇总</t>
   </si>
   <si>
-    <t>2023年 08月 01日至2023年 08月 31日</t>
+    <t>2023年 10月 01日至2023年 10月 31日</t>
   </si>
   <si>
     <t>编辑</t>
@@ -62,16 +62,16 @@
     <t>黄礼闯</t>
   </si>
   <si>
-    <t>BI2023072101</t>
+    <t>夏国连生信支持</t>
   </si>
   <si>
     <t>固定业务</t>
   </si>
   <si>
-    <t>3-5</t>
-  </si>
-  <si>
-    <t>结合 scRNA-seq 和 bulk RNA-seq 探究昼夜节律基因对于 ccRCC 的预后评估价值</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>筛选丹参酮治疗脓毒症的关键差异表达基因及相关信号通路</t>
   </si>
   <si>
     <t>完成</t>
@@ -80,19 +80,79 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>IN2023072803</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>筛出（瘢痕增生）能够与 TCF-AS1 结合又能与 TCF4 结合的 RNA 结合蛋白</t>
-  </si>
-  <si>
-    <t>沈顺订单：结合网络药理、16s rRNA、代谢组分析中药复方对糖尿病肾病的作用和靶点（分两部分）</t>
-  </si>
-  <si>
-    <t>完成第一部分</t>
+    <t>曹卓空间转录组</t>
+  </si>
+  <si>
+    <t>癌细胞鉴定、亚群鉴定、marker分析、细胞通讯等。</t>
+  </si>
+  <si>
+    <t>修改业务</t>
+  </si>
+  <si>
+    <t>重新评估需要修改的地方，然后对文章进行修改</t>
+  </si>
+  <si>
+    <t>BI2023080108</t>
+  </si>
+  <si>
+    <t>慢性肾病和肾癌的关联分析（题目待定）</t>
+  </si>
+  <si>
+    <t>待完成</t>
+  </si>
+  <si>
+    <t>李华评估</t>
+  </si>
+  <si>
+    <t>评估业务</t>
+  </si>
+  <si>
+    <t>李华评估，了解系统性硬化症 Systemic Sclerosis 开源数据库现状。</t>
+  </si>
+  <si>
+    <t>周芳评估</t>
+  </si>
+  <si>
+    <t>周芳评估，设计关于特应性皮炎 Atopic Dermatitis 5分以上生信。</t>
+  </si>
+  <si>
+    <t>袁路评估</t>
+  </si>
+  <si>
+    <t>袁路评估，糖尿病视网膜病变与眼底图像的计量分析的可行性。</t>
+  </si>
+  <si>
+    <t>袁路加急评估</t>
+  </si>
+  <si>
+    <t>袁路加急评估，文献计量的图表可否实现。</t>
+  </si>
+  <si>
+    <t>贾总晓月评估</t>
+  </si>
+  <si>
+    <t>贾总晓月评估，联合三维基因组测序与单细胞测序技术的分析实现可行性。</t>
+  </si>
+  <si>
+    <t>方和敬生信支持</t>
+  </si>
+  <si>
+    <t>方和敬生信支持，网络药理学涉及白茅根和王不留行的药物-成分-靶点分析。</t>
+  </si>
+  <si>
+    <t>夏国连补充分析</t>
+  </si>
+  <si>
+    <t>夏国连补充分析，将分析结果与跟肠道微生物和免疫微环境相关相联系。</t>
+  </si>
+  <si>
+    <t>夏国连补充分析，寻找铁死亡相关的基因或通路。</t>
+  </si>
+  <si>
+    <t>业务审核</t>
+  </si>
+  <si>
+    <t>孙楠的十个业务单和温呈金的一个业务单</t>
   </si>
   <si>
     <t>汇总表</t>
@@ -939,6 +999,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -955,6 +1022,67 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -964,7 +1092,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -977,39 +1105,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1023,27 +1120,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1053,23 +1129,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1155,7 +1215,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1167,7 +1239,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1179,7 +1287,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1191,49 +1347,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1246,84 +1384,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1422,11 +1482,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1457,6 +1538,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1465,188 +1555,158 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1656,7 +1716,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1771,9 +1831,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1815,8 +1872,8 @@
   </cellXfs>
   <cellStyles count="56">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2 2 2 2" xfId="1"/>
-    <cellStyle name="常规 14 2 2" xfId="2"/>
+    <cellStyle name="常规 14 2 2" xfId="1"/>
+    <cellStyle name="常规 2 2 2 2" xfId="2"/>
     <cellStyle name="60% - Accent6" xfId="3" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
@@ -1886,14 +1943,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1902,7 +1959,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1781175" y="4257675"/>
+          <a:off x="1781175" y="4539615"/>
           <a:ext cx="13506450" cy="2781300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1946,7 +2003,7 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -1962,8 +2019,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10182225" y="3267075"/>
-          <a:ext cx="2019300" cy="533400"/>
+          <a:off x="10182225" y="3457575"/>
+          <a:ext cx="2019300" cy="342900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2019,7 +2076,7 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1514475</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -2035,8 +2092,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10753725" y="3857625"/>
-          <a:ext cx="323850" cy="581025"/>
+          <a:off x="10753725" y="4238625"/>
+          <a:ext cx="323850" cy="200025"/>
         </a:xfrm>
         <a:prstGeom prst="upArrow">
           <a:avLst/>
@@ -2361,8 +2418,8 @@
   <sheetPr/>
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2481,12 +2538,10 @@
       <c r="I7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="49" t="s">
+      <c r="J7" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="23">
-        <v>0.34</v>
-      </c>
+      <c r="K7" s="23"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="23" t="s">
@@ -2502,20 +2557,18 @@
         <v>16</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="39"/>
       <c r="I8" s="23" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="23"/>
-      <c r="K8" s="23">
-        <v>0.33</v>
-      </c>
+      <c r="K8" s="23"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="23" t="s">
@@ -2524,12 +2577,14 @@
       <c r="B9" s="23">
         <v>3</v>
       </c>
-      <c r="C9" s="23"/>
+      <c r="C9" s="23">
+        <v>2023041204</v>
+      </c>
       <c r="D9" s="23" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="38" t="s">
@@ -2537,92 +2592,309 @@
       </c>
       <c r="H9" s="39"/>
       <c r="I9" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="23">
+        <v>4</v>
+      </c>
+      <c r="C10" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
+      <c r="D10" s="23" t="s">
+        <v>16</v>
+      </c>
       <c r="E10" s="37"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="38"/>
+      <c r="G10" s="38" t="s">
+        <v>26</v>
+      </c>
       <c r="H10" s="39"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="49"/>
+      <c r="I10" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="48"/>
       <c r="K10" s="23"/>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-    </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="23"/>
+      <c r="A12" s="23" t="s">
+        <v>14</v>
+      </c>
       <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="37"/>
+      <c r="C12" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="23"/>
       <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
+      <c r="G12" s="23" t="s">
+        <v>30</v>
+      </c>
       <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
+      <c r="I12" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="J12" s="23"/>
       <c r="K12" s="23"/>
     </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+    </row>
     <row r="26" spans="4:4">
       <c r="D26" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="4:11">
       <c r="D27" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="41" t="s">
-        <v>28</v>
+        <v>47</v>
+      </c>
+      <c r="E27" s="40" t="s">
+        <v>48</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="G27" s="42" t="s">
-        <v>30</v>
+        <v>49</v>
+      </c>
+      <c r="G27" s="41" t="s">
+        <v>50</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="I27" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="J27" s="51" t="s">
-        <v>33</v>
-      </c>
-      <c r="K27" s="51" t="s">
-        <v>34</v>
+        <v>51</v>
+      </c>
+      <c r="I27" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="J27" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="K27" s="50" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="4:11">
       <c r="D28" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="44" t="s">
-        <v>37</v>
+        <v>55</v>
+      </c>
+      <c r="E28" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="43" t="s">
+        <v>57</v>
       </c>
       <c r="G28" s="26">
         <v>4.2</v>
@@ -2630,41 +2902,41 @@
       <c r="H28" s="26">
         <v>1.1</v>
       </c>
-      <c r="I28" s="52" t="s">
-        <v>38</v>
+      <c r="I28" s="51" t="s">
+        <v>58</v>
       </c>
       <c r="J28" s="26"/>
-      <c r="K28" s="53"/>
+      <c r="K28" s="52"/>
     </row>
     <row r="29" spans="4:11">
       <c r="D29" s="26"/>
-      <c r="E29" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" s="44" t="s">
-        <v>40</v>
+      <c r="E29" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="43" t="s">
+        <v>60</v>
       </c>
       <c r="G29" s="26" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="H29" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="I29" s="52" t="s">
-        <v>43</v>
+        <v>62</v>
+      </c>
+      <c r="I29" s="51" t="s">
+        <v>63</v>
       </c>
       <c r="J29" s="26"/>
-      <c r="K29" s="53"/>
+      <c r="K29" s="52"/>
     </row>
     <row r="30" spans="4:11">
       <c r="D30" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E30" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="F30" s="44" t="s">
-        <v>37</v>
+        <v>64</v>
+      </c>
+      <c r="E30" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="43" t="s">
+        <v>57</v>
       </c>
       <c r="G30" s="26">
         <v>4</v>
@@ -2672,76 +2944,76 @@
       <c r="H30" s="26">
         <v>1</v>
       </c>
-      <c r="I30" s="52" t="s">
-        <v>45</v>
+      <c r="I30" s="51" t="s">
+        <v>65</v>
       </c>
       <c r="J30" s="26"/>
-      <c r="K30" s="54"/>
+      <c r="K30" s="53"/>
     </row>
     <row r="31" spans="4:11">
       <c r="D31" s="26"/>
-      <c r="E31" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" s="44" t="s">
-        <v>40</v>
+      <c r="E31" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="43" t="s">
+        <v>60</v>
       </c>
       <c r="G31" s="26" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="H31" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="I31" s="52" t="s">
-        <v>43</v>
+        <v>62</v>
+      </c>
+      <c r="I31" s="51" t="s">
+        <v>63</v>
       </c>
       <c r="J31" s="26"/>
-      <c r="K31" s="54"/>
+      <c r="K31" s="53"/>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="27" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="28" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="B37" s="28"/>
       <c r="C37" s="28"/>
       <c r="D37" s="28"/>
-      <c r="E37" s="46"/>
+      <c r="E37" s="45"/>
     </row>
     <row r="38" ht="15.75" spans="1:7">
       <c r="A38" s="29" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="B38" s="29"/>
       <c r="C38" s="29"/>
       <c r="D38" s="29"/>
-      <c r="E38" s="47"/>
+      <c r="E38" s="46"/>
       <c r="F38" s="29"/>
       <c r="G38" s="29"/>
     </row>
     <row r="39" ht="15.75" spans="1:7">
       <c r="A39" s="29" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
       <c r="D39" s="29"/>
-      <c r="E39" s="47"/>
+      <c r="E39" s="46"/>
       <c r="F39" s="29"/>
       <c r="G39" s="29"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="30" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B40" s="31"/>
       <c r="C40" s="31"/>
       <c r="D40" s="31"/>
-      <c r="E40" s="48"/>
+      <c r="E40" s="47"/>
       <c r="F40" s="31"/>
       <c r="G40" s="31"/>
     </row>
@@ -2793,7 +3065,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2837,7 +3109,7 @@
     </row>
     <row r="3" ht="23.25" spans="1:19">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2860,11 +3132,11 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -2875,33 +3147,33 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="P5" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="M5" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>35</v>
-      </c>
       <c r="Q5" s="11" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" ht="28.5" customHeight="1" spans="1:19">
       <c r="A6" s="4" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -2926,16 +3198,16 @@
         <v>0.01</v>
       </c>
       <c r="P6" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="Q6" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="R6" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="S6" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -2963,16 +3235,16 @@
         <v>0.01</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="R7" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="S7" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -3000,16 +3272,16 @@
         <v>0.01</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="Q8" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="R8" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="S8" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -3037,22 +3309,22 @@
         <v>0.01</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="Q9" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="R9" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="S9" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1" spans="1:19">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
@@ -3076,21 +3348,21 @@
         <v>0.01</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="Q10" s="18" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="R10" s="18" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="S10" s="18" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="4" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -3115,21 +3387,21 @@
         <v>0.05</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="Q11" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="R11" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="S11" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="9" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -3154,16 +3426,16 @@
         <v>0.95</v>
       </c>
       <c r="P12" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="Q12" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="R12" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="S12" s="18" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tue Oct 31 06:50:04 AM CST 2023
</commit_message>
<xml_diff>
--- a/lixiao/performance_2023_10/assess_绩效+软性考核表.xlsx
+++ b/lixiao/performance_2023_10/assess_绩效+软性考核表.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="88">
   <si>
     <t>绩效考核汇总</t>
   </si>
@@ -86,21 +86,21 @@
     <t>癌细胞鉴定、亚群鉴定、marker分析、细胞通讯等。</t>
   </si>
   <si>
+    <t>BI2023080108</t>
+  </si>
+  <si>
+    <t>慢性肾病和肾癌的关联分析（题目待定）</t>
+  </si>
+  <si>
+    <t>待完成</t>
+  </si>
+  <si>
     <t>修改业务</t>
   </si>
   <si>
     <t>重新评估需要修改的地方，然后对文章进行修改</t>
   </si>
   <si>
-    <t>BI2023080108</t>
-  </si>
-  <si>
-    <t>慢性肾病和肾癌的关联分析（题目待定）</t>
-  </si>
-  <si>
-    <t>待完成</t>
-  </si>
-  <si>
     <t>李华评估</t>
   </si>
   <si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>夏国连补充分析，将分析结果与跟肠道微生物和免疫微环境相关相联系。</t>
+  </si>
+  <si>
+    <t>评估业务合计：</t>
   </si>
   <si>
     <t>夏国连补充分析，寻找铁死亡相关的基因或通路。</t>
@@ -908,10 +911,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="37">
     <font>
@@ -999,10 +1002,124 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1014,90 +1131,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1105,39 +1138,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1215,19 +1218,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1239,7 +1230,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1257,7 +1266,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1269,19 +1302,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1293,97 +1386,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1458,26 +1461,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1514,24 +1517,35 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1544,179 +1558,168 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1785,6 +1788,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1831,6 +1837,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1856,6 +1871,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="17" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1872,8 +1890,8 @@
   </cellXfs>
   <cellStyles count="56">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 14 2 2" xfId="1"/>
-    <cellStyle name="常规 2 2 2 2" xfId="2"/>
+    <cellStyle name="常规 2 2 2 2" xfId="1"/>
+    <cellStyle name="常规 14 2 2" xfId="2"/>
     <cellStyle name="60% - Accent6" xfId="3" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
@@ -1943,13 +1961,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
@@ -1959,8 +1977,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1781175" y="4539615"/>
-          <a:ext cx="13506450" cy="2781300"/>
+          <a:off x="1781175" y="4730115"/>
+          <a:ext cx="13668375" cy="2781300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2003,13 +2021,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
@@ -2019,7 +2037,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10182225" y="3457575"/>
+          <a:off x="10182225" y="3648075"/>
           <a:ext cx="2019300" cy="342900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2076,13 +2094,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1514475</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1838325</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
@@ -2092,7 +2110,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10753725" y="4238625"/>
+          <a:off x="10753725" y="4429125"/>
           <a:ext cx="323850" cy="200025"/>
         </a:xfrm>
         <a:prstGeom prst="upArrow">
@@ -2416,10 +2434,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2432,6 +2450,7 @@
     <col min="7" max="8" width="29.375" customWidth="1"/>
     <col min="9" max="9" width="33.5" customWidth="1"/>
     <col min="10" max="10" width="27.5" customWidth="1"/>
+    <col min="11" max="11" width="11.125"/>
   </cols>
   <sheetData>
     <row r="1" ht="33" customHeight="1" spans="1:11">
@@ -2441,7 +2460,7 @@
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
-      <c r="E1" s="32"/>
+      <c r="E1" s="33"/>
       <c r="F1" s="20"/>
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
@@ -2456,7 +2475,7 @@
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
-      <c r="E3" s="33"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
@@ -2477,16 +2496,16 @@
       <c r="D5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="35" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="35"/>
+      <c r="H5" s="36"/>
       <c r="I5" s="22" t="s">
         <v>9</v>
       </c>
@@ -2502,12 +2521,12 @@
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
-      <c r="E6" s="34"/>
+      <c r="E6" s="35"/>
       <c r="F6" s="22"/>
       <c r="G6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="37" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="22"/>
@@ -2527,21 +2546,23 @@
       <c r="D7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="38" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="23"/>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="39"/>
+      <c r="H7" s="40"/>
       <c r="I7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="48" t="s">
+      <c r="J7" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="23"/>
+      <c r="K7" s="23">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="23" t="s">
@@ -2556,19 +2577,21 @@
       <c r="D8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="38" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="23"/>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="39"/>
+      <c r="H8" s="40"/>
       <c r="I8" s="23" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
+      <c r="K8" s="23">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="23" t="s">
@@ -2577,73 +2600,65 @@
       <c r="B9" s="23">
         <v>3</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="38"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="40"/>
+      <c r="I9" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="52"/>
+      <c r="K9" s="23">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23">
         <v>2023041204</v>
       </c>
-      <c r="D9" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="37" t="s">
+      <c r="D11" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="39"/>
-      <c r="I9" s="23" t="s">
+      <c r="F11" s="23"/>
+      <c r="G11" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="40"/>
+      <c r="I11" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="23">
-        <v>4</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="39"/>
-      <c r="I10" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="48"/>
-      <c r="K10" s="23"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23">
+        <v>0.083</v>
+      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="23" t="s">
@@ -2651,7 +2666,7 @@
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>29</v>
@@ -2659,7 +2674,7 @@
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
       <c r="G13" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H13" s="23"/>
       <c r="I13" s="23" t="s">
@@ -2674,7 +2689,7 @@
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>29</v>
@@ -2682,7 +2697,7 @@
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
       <c r="G14" s="23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H14" s="23"/>
       <c r="I14" s="23" t="s">
@@ -2697,7 +2712,7 @@
       </c>
       <c r="B15" s="23"/>
       <c r="C15" s="23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>29</v>
@@ -2705,7 +2720,7 @@
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
       <c r="G15" s="23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H15" s="23"/>
       <c r="I15" s="23" t="s">
@@ -2720,7 +2735,7 @@
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>29</v>
@@ -2728,7 +2743,7 @@
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H16" s="23"/>
       <c r="I16" s="23" t="s">
@@ -2743,7 +2758,7 @@
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="23" t="s">
         <v>29</v>
@@ -2751,7 +2766,7 @@
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H17" s="23"/>
       <c r="I17" s="23" t="s">
@@ -2766,7 +2781,7 @@
       </c>
       <c r="B18" s="23"/>
       <c r="C18" s="23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" s="23" t="s">
         <v>29</v>
@@ -2774,7 +2789,7 @@
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H18" s="23"/>
       <c r="I18" s="23" t="s">
@@ -2797,52 +2812,68 @@
       <c r="E19" s="23"/>
       <c r="F19" s="23"/>
       <c r="G19" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H19" s="23"/>
       <c r="I19" s="23" t="s">
         <v>19</v>
       </c>
       <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="23" t="s">
+      <c r="K19" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23" t="s">
+      <c r="B20" s="23"/>
+      <c r="C20" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="H20" s="23"/>
+      <c r="I20" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="23"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
+      <c r="G22" s="23" t="s">
+        <v>46</v>
+      </c>
       <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
+      <c r="I22" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="K22" s="23">
+        <v>0.092</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="23"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
@@ -2853,193 +2884,205 @@
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
       <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-    </row>
-    <row r="26" spans="4:4">
-      <c r="D26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="4:11">
-      <c r="D27" s="24" t="s">
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+    </row>
+    <row r="27" spans="4:4">
+      <c r="D27" t="s">
         <v>47</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="F27" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="G27" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="H27" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="I27" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="J27" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="K27" s="50" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="28" spans="4:11">
       <c r="D28" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="I28" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="J28" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="K28" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="42" t="s">
+    </row>
+    <row r="29" spans="4:11">
+      <c r="D29" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="F28" s="43" t="s">
+      <c r="E29" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="G28" s="26">
+      <c r="F29" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="27">
         <v>4.2</v>
       </c>
-      <c r="H28" s="26">
+      <c r="H29" s="27">
         <v>1.1</v>
       </c>
-      <c r="I28" s="51" t="s">
+      <c r="I29" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="J29" s="27"/>
+      <c r="K29" s="57"/>
+    </row>
+    <row r="30" spans="4:11">
+      <c r="D30" s="27"/>
+      <c r="E30" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="I30" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="J30" s="27"/>
+      <c r="K30" s="57"/>
+    </row>
+    <row r="31" spans="4:11">
+      <c r="D31" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="J28" s="26"/>
-      <c r="K28" s="52"/>
-    </row>
-    <row r="29" spans="4:11">
-      <c r="D29" s="26"/>
-      <c r="E29" s="44" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29" s="43" t="s">
+      <c r="G31" s="27">
+        <v>4</v>
+      </c>
+      <c r="H31" s="27">
+        <v>1</v>
+      </c>
+      <c r="I31" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="J31" s="27"/>
+      <c r="K31" s="58"/>
+    </row>
+    <row r="32" spans="4:11">
+      <c r="D32" s="27"/>
+      <c r="E32" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="G29" s="26" t="s">
+      <c r="F32" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="H29" s="26" t="s">
+      <c r="G32" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="I29" s="51" t="s">
+      <c r="H32" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="J29" s="26"/>
-      <c r="K29" s="52"/>
-    </row>
-    <row r="30" spans="4:11">
-      <c r="D30" s="25" t="s">
+      <c r="I32" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="E30" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="G30" s="26">
-        <v>4</v>
-      </c>
-      <c r="H30" s="26">
-        <v>1</v>
-      </c>
-      <c r="I30" s="51" t="s">
-        <v>65</v>
-      </c>
-      <c r="J30" s="26"/>
-      <c r="K30" s="53"/>
-    </row>
-    <row r="31" spans="4:11">
-      <c r="D31" s="26"/>
-      <c r="E31" s="44" t="s">
-        <v>59</v>
-      </c>
-      <c r="F31" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="G31" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="H31" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="I31" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="J31" s="26"/>
-      <c r="K31" s="53"/>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="J32" s="27"/>
+      <c r="K32" s="58"/>
+    </row>
+    <row r="37" spans="1:1">
       <c r="A37" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="45"/>
-    </row>
-    <row r="38" ht="15.75" spans="1:7">
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="29" t="s">
         <v>68</v>
       </c>
       <c r="B38" s="29"/>
       <c r="C38" s="29"/>
       <c r="D38" s="29"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
+      <c r="E38" s="49"/>
     </row>
     <row r="39" ht="15.75" spans="1:7">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+    </row>
+    <row r="40" ht="15.75" spans="1:7">
       <c r="A40" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="21">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="A38:G38"/>
     <mergeCell ref="A39:G39"/>
     <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A41:G41"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D31:D32"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="J31:J32"/>
     <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="K31:K32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3065,7 +3108,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3109,7 +3152,7 @@
     </row>
     <row r="3" ht="23.25" spans="1:19">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -3132,11 +3175,11 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -3147,33 +3190,33 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N5" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" ht="28.5" customHeight="1" spans="1:19">
       <c r="A6" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
@@ -3198,16 +3241,16 @@
         <v>0.01</v>
       </c>
       <c r="P6" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q6" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="R6" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="S6" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -3235,16 +3278,16 @@
         <v>0.01</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="R7" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="S7" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -3272,16 +3315,16 @@
         <v>0.01</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q8" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="R8" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="S8" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -3309,22 +3352,22 @@
         <v>0.01</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q9" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="R9" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="S9" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1" spans="1:19">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
@@ -3348,21 +3391,21 @@
         <v>0.01</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="Q10" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="R10" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="S10" s="18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -3387,21 +3430,21 @@
         <v>0.05</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q11" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="R11" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="S11" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -3426,16 +3469,16 @@
         <v>0.95</v>
       </c>
       <c r="P12" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q12" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="R12" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="S12" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>